<commit_message>
Adjusted all example setup template files with new  field
</commit_message>
<xml_diff>
--- a/Example_Files/Template; Compound Setup Table 8K Up to 32 Compunds 10 Point Dose.xlsx
+++ b/Example_Files/Template; Compound Setup Table 8K Up to 32 Compunds 10 Point Dose.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bfulroth/GitProjects/SPR_Create_Dotmatics_ADLP_File/Example Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bfulroth/GitProjects/SPR_Create_Dotmatics_ADLP_File/Example_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64624793-DE30-3F41-90BE-BB5E9348DC10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AD080A-961F-824A-9FA5-C7DC78A40C5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Table 1-1-1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
   <si>
     <t>Broad ID</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t>P24</t>
+  </si>
+  <si>
+    <t>Plate_Barcode</t>
   </si>
 </sst>
 </file>
@@ -1973,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:IU33"/>
+  <dimension ref="A1:IV33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -1985,13 +1988,15 @@
     <col min="2" max="2" width="26.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="11" width="11.33203125" style="1" customWidth="1"/>
-    <col min="12" max="16" width="10.83203125" style="1" customWidth="1"/>
-    <col min="17" max="18" width="17.83203125" style="1" customWidth="1"/>
-    <col min="19" max="255" width="10.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="1" customWidth="1"/>
+    <col min="7" max="12" width="11.33203125" style="1" customWidth="1"/>
+    <col min="13" max="17" width="10.83203125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="17.83203125" style="1" customWidth="1"/>
+    <col min="20" max="256" width="10.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.75" customHeight="1">
+    <row r="1" spans="1:19" ht="14.75" customHeight="1">
       <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
@@ -2007,47 +2012,50 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="N1" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="O1" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="57" t="s">
+      <c r="P1" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -2061,51 +2069,52 @@
       <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="7">
-        <v>1206274707</v>
-      </c>
+      <c r="F2" s="6"/>
       <c r="G2" s="7">
         <v>1206274707</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7">
+        <v>1206274707</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="7">
-        <v>10</v>
-      </c>
-      <c r="J2" s="9">
-        <f>I2*1000</f>
+      <c r="J2" s="7">
+        <v>10</v>
+      </c>
+      <c r="K2" s="9">
+        <f>J2*1000</f>
         <v>10000</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="9">
+      <c r="M2" s="9">
         <v>200</v>
       </c>
-      <c r="M2" s="9">
+      <c r="N2" s="9">
         <v>50</v>
       </c>
-      <c r="N2" s="9">
+      <c r="O2" s="9">
         <v>2</v>
       </c>
-      <c r="O2" s="7">
-        <v>10</v>
-      </c>
       <c r="P2" s="7">
-        <f t="shared" ref="P2:P33" si="0">L2-Q2-R2</f>
+        <v>10</v>
+      </c>
+      <c r="Q2" s="7">
+        <f t="shared" ref="Q2:Q33" si="0">M2-R2-S2</f>
         <v>190</v>
       </c>
-      <c r="Q2" s="11">
-        <f t="shared" ref="Q2:Q33" si="1">(M2*L2)/J2</f>
+      <c r="R2" s="11">
+        <f t="shared" ref="R2:R33" si="1">(N2*M2)/K2</f>
         <v>1</v>
       </c>
-      <c r="R2" s="12">
-        <f t="shared" ref="R2:R33" si="2">10-Q2</f>
+      <c r="S2" s="12">
+        <f t="shared" ref="S2:S33" si="2">10-R2</f>
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:19">
       <c r="A3" s="13" t="s">
         <v>23</v>
       </c>
@@ -2119,50 +2128,51 @@
       <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="15">
-        <v>1196295332</v>
-      </c>
+      <c r="F3" s="14"/>
       <c r="G3" s="15">
         <v>1196295332</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="15">
+        <v>1196295332</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="15">
-        <v>10</v>
-      </c>
-      <c r="J3" s="17">
+      <c r="J3" s="15">
+        <v>10</v>
+      </c>
+      <c r="K3" s="17">
         <v>10000</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="L3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="17">
+      <c r="M3" s="17">
         <v>200</v>
       </c>
-      <c r="M3" s="17">
+      <c r="N3" s="17">
         <v>20</v>
       </c>
-      <c r="N3" s="17">
+      <c r="O3" s="17">
         <v>2</v>
       </c>
-      <c r="O3" s="15">
-        <v>10</v>
-      </c>
       <c r="P3" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q3" s="19">
+      <c r="R3" s="19">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="R3" s="20">
+      <c r="S3" s="20">
         <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4" s="13" t="s">
         <v>28</v>
       </c>
@@ -2176,50 +2186,51 @@
       <c r="E4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="22">
-        <v>1196295245</v>
-      </c>
+      <c r="F4" s="21"/>
       <c r="G4" s="22">
         <v>1196295245</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="22">
+        <v>1196295245</v>
+      </c>
+      <c r="I4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="15">
-        <v>10</v>
-      </c>
-      <c r="J4" s="17">
+      <c r="J4" s="15">
+        <v>10</v>
+      </c>
+      <c r="K4" s="17">
         <v>10000</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="L4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="17">
+      <c r="M4" s="17">
         <v>200</v>
       </c>
-      <c r="M4" s="17">
+      <c r="N4" s="17">
         <v>20</v>
       </c>
-      <c r="N4" s="17">
+      <c r="O4" s="17">
         <v>2</v>
       </c>
-      <c r="O4" s="15">
-        <v>10</v>
-      </c>
       <c r="P4" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="R4" s="19">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="R4" s="20">
+      <c r="S4" s="20">
         <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" s="13" t="s">
         <v>31</v>
       </c>
@@ -2233,50 +2244,51 @@
       <c r="E5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="15">
-        <v>1196295253</v>
-      </c>
+      <c r="F5" s="14"/>
       <c r="G5" s="15">
         <v>1196295253</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="15">
+        <v>1196295253</v>
+      </c>
+      <c r="I5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="15">
-        <v>10</v>
-      </c>
-      <c r="J5" s="17">
+      <c r="J5" s="15">
+        <v>10</v>
+      </c>
+      <c r="K5" s="17">
         <v>10000</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="L5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="17">
+      <c r="M5" s="17">
         <v>200</v>
       </c>
-      <c r="M5" s="17">
+      <c r="N5" s="17">
         <v>20</v>
       </c>
-      <c r="N5" s="17">
+      <c r="O5" s="17">
         <v>2</v>
       </c>
-      <c r="O5" s="15">
-        <v>10</v>
-      </c>
       <c r="P5" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="R5" s="19">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="R5" s="20">
+      <c r="S5" s="20">
         <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" s="13" t="s">
         <v>34</v>
       </c>
@@ -2290,50 +2302,51 @@
       <c r="E6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="15">
-        <v>1196295261</v>
-      </c>
+      <c r="F6" s="14"/>
       <c r="G6" s="15">
         <v>1196295261</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="15">
+        <v>1196295261</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="15">
-        <v>10</v>
-      </c>
-      <c r="J6" s="17">
+      <c r="J6" s="15">
+        <v>10</v>
+      </c>
+      <c r="K6" s="17">
         <v>10000</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="L6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="17">
+      <c r="M6" s="17">
         <v>200</v>
       </c>
-      <c r="M6" s="17">
+      <c r="N6" s="17">
         <v>20</v>
       </c>
-      <c r="N6" s="17">
+      <c r="O6" s="17">
         <v>2</v>
       </c>
-      <c r="O6" s="15">
-        <v>10</v>
-      </c>
       <c r="P6" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="R6" s="19">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="R6" s="20">
+      <c r="S6" s="20">
         <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7" s="13" t="s">
         <v>18</v>
       </c>
@@ -2347,51 +2360,52 @@
       <c r="E7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="15">
-        <v>1206274707</v>
-      </c>
+      <c r="F7" s="14"/>
       <c r="G7" s="15">
         <v>1206274707</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="15">
+        <v>1206274707</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="15">
-        <v>10</v>
-      </c>
-      <c r="J7" s="17">
-        <f>I7*1000</f>
+      <c r="J7" s="15">
+        <v>10</v>
+      </c>
+      <c r="K7" s="17">
+        <f>J7*1000</f>
         <v>10000</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="L7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="17">
+      <c r="M7" s="17">
         <v>200</v>
       </c>
-      <c r="M7" s="17">
+      <c r="N7" s="17">
         <v>20</v>
       </c>
-      <c r="N7" s="17">
+      <c r="O7" s="17">
         <v>2</v>
       </c>
-      <c r="O7" s="15">
-        <v>10</v>
-      </c>
       <c r="P7" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q7" s="19">
+      <c r="R7" s="19">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="R7" s="20">
+      <c r="S7" s="20">
         <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:19">
       <c r="A8" s="13" t="s">
         <v>38</v>
       </c>
@@ -2405,50 +2419,51 @@
       <c r="E8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="15">
-        <v>1196295269</v>
-      </c>
+      <c r="F8" s="14"/>
       <c r="G8" s="15">
         <v>1196295269</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15">
+        <v>1196295269</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="15">
-        <v>10</v>
-      </c>
-      <c r="J8" s="17">
+      <c r="J8" s="15">
+        <v>10</v>
+      </c>
+      <c r="K8" s="17">
         <v>10000</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="L8" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="17">
+      <c r="M8" s="17">
         <v>200</v>
       </c>
-      <c r="M8" s="17">
+      <c r="N8" s="17">
         <v>50</v>
       </c>
-      <c r="N8" s="17">
+      <c r="O8" s="17">
         <v>2</v>
       </c>
-      <c r="O8" s="15">
-        <v>10</v>
-      </c>
       <c r="P8" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q8" s="19">
+      <c r="R8" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R8" s="20">
+      <c r="S8" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:19">
       <c r="A9" s="23" t="s">
         <v>40</v>
       </c>
@@ -2462,51 +2477,52 @@
       <c r="E9" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="25">
-        <v>1196295277</v>
-      </c>
+      <c r="F9" s="24"/>
       <c r="G9" s="25">
         <v>1196295277</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="25">
+        <v>1196295277</v>
+      </c>
+      <c r="I9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="25">
-        <v>10</v>
-      </c>
-      <c r="J9" s="27">
-        <f>I9*1000</f>
+      <c r="J9" s="25">
+        <v>10</v>
+      </c>
+      <c r="K9" s="27">
+        <f>J9*1000</f>
         <v>10000</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="L9" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="27">
+      <c r="M9" s="27">
         <v>200</v>
       </c>
-      <c r="M9" s="27">
+      <c r="N9" s="27">
         <v>50</v>
       </c>
-      <c r="N9" s="27">
+      <c r="O9" s="27">
         <v>2</v>
       </c>
-      <c r="O9" s="25">
-        <v>10</v>
-      </c>
       <c r="P9" s="25">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="25">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q9" s="29">
+      <c r="R9" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R9" s="30">
+      <c r="S9" s="30">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:19">
       <c r="A10" s="5" t="s">
         <v>43</v>
       </c>
@@ -2520,50 +2536,51 @@
       <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="7">
-        <v>1196295474</v>
-      </c>
+      <c r="F10" s="6"/>
       <c r="G10" s="7">
         <v>1196295474</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="7">
+        <v>1196295474</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="7">
-        <v>10</v>
-      </c>
-      <c r="J10" s="9">
+      <c r="J10" s="7">
+        <v>10</v>
+      </c>
+      <c r="K10" s="9">
         <v>10000</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="L10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="9">
+      <c r="M10" s="9">
         <v>200</v>
       </c>
-      <c r="M10" s="9">
+      <c r="N10" s="9">
         <v>50</v>
       </c>
-      <c r="N10" s="9">
+      <c r="O10" s="9">
         <v>2</v>
       </c>
-      <c r="O10" s="7">
-        <v>10</v>
-      </c>
       <c r="P10" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="7">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q10" s="11">
+      <c r="R10" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R10" s="12">
+      <c r="S10" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:19">
       <c r="A11" s="13" t="s">
         <v>46</v>
       </c>
@@ -2575,50 +2592,51 @@
       <c r="E11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="22">
-        <v>1196295482</v>
-      </c>
+      <c r="F11" s="21"/>
       <c r="G11" s="22">
         <v>1196295482</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="22">
+        <v>1196295482</v>
+      </c>
+      <c r="I11" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="15">
-        <v>10</v>
-      </c>
-      <c r="J11" s="17">
+      <c r="J11" s="15">
+        <v>10</v>
+      </c>
+      <c r="K11" s="17">
         <v>10000</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="L11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="L11" s="17">
+      <c r="M11" s="17">
         <v>200</v>
       </c>
-      <c r="M11" s="17">
+      <c r="N11" s="17">
         <v>50</v>
       </c>
-      <c r="N11" s="17">
+      <c r="O11" s="17">
         <v>2</v>
       </c>
-      <c r="O11" s="15">
-        <v>10</v>
-      </c>
       <c r="P11" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q11" s="19">
+      <c r="R11" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R11" s="20">
+      <c r="S11" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:19">
       <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
@@ -2632,51 +2650,52 @@
       <c r="E12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="15">
-        <v>1206274707</v>
-      </c>
+      <c r="F12" s="14"/>
       <c r="G12" s="15">
         <v>1206274707</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="15">
+        <v>1206274707</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="15">
-        <v>10</v>
-      </c>
-      <c r="J12" s="17">
-        <f>I12*1000</f>
+      <c r="J12" s="15">
+        <v>10</v>
+      </c>
+      <c r="K12" s="17">
+        <f>J12*1000</f>
         <v>10000</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="L12" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="17">
+      <c r="M12" s="17">
         <v>200</v>
       </c>
-      <c r="M12" s="17">
+      <c r="N12" s="17">
         <v>50</v>
       </c>
-      <c r="N12" s="17">
+      <c r="O12" s="17">
         <v>2</v>
       </c>
-      <c r="O12" s="15">
-        <v>10</v>
-      </c>
       <c r="P12" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="R12" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R12" s="20">
+      <c r="S12" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:19">
       <c r="A13" s="13" t="s">
         <v>50</v>
       </c>
@@ -2688,50 +2707,51 @@
       <c r="E13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="22">
-        <v>1196295490</v>
-      </c>
+      <c r="F13" s="21"/>
       <c r="G13" s="22">
         <v>1196295490</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="22">
+        <v>1196295490</v>
+      </c>
+      <c r="I13" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="15">
-        <v>10</v>
-      </c>
-      <c r="J13" s="17">
+      <c r="J13" s="15">
+        <v>10</v>
+      </c>
+      <c r="K13" s="17">
         <v>10000</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="L13" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="17">
+      <c r="M13" s="17">
         <v>200</v>
       </c>
-      <c r="M13" s="17">
+      <c r="N13" s="17">
         <v>50</v>
       </c>
-      <c r="N13" s="17">
+      <c r="O13" s="17">
         <v>2</v>
       </c>
-      <c r="O13" s="15">
-        <v>10</v>
-      </c>
       <c r="P13" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q13" s="19">
+      <c r="R13" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R13" s="20">
+      <c r="S13" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:19">
       <c r="A14" s="13" t="s">
         <v>53</v>
       </c>
@@ -2743,50 +2763,51 @@
       <c r="E14" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="22">
-        <v>1196295522</v>
-      </c>
+      <c r="F14" s="21"/>
       <c r="G14" s="22">
         <v>1196295522</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="22">
+        <v>1196295522</v>
+      </c>
+      <c r="I14" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="15">
-        <v>10</v>
-      </c>
-      <c r="J14" s="17">
+      <c r="J14" s="15">
+        <v>10</v>
+      </c>
+      <c r="K14" s="17">
         <v>10000</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="L14" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="L14" s="17">
+      <c r="M14" s="17">
         <v>200</v>
       </c>
-      <c r="M14" s="17">
+      <c r="N14" s="17">
         <v>50</v>
       </c>
-      <c r="N14" s="17">
+      <c r="O14" s="17">
         <v>2</v>
       </c>
-      <c r="O14" s="15">
-        <v>10</v>
-      </c>
       <c r="P14" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q14" s="19">
+      <c r="R14" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R14" s="20">
+      <c r="S14" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:19">
       <c r="A15" s="13" t="s">
         <v>56</v>
       </c>
@@ -2798,50 +2819,51 @@
       <c r="E15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="22">
-        <v>1196295506</v>
-      </c>
+      <c r="F15" s="21"/>
       <c r="G15" s="22">
         <v>1196295506</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="22">
+        <v>1196295506</v>
+      </c>
+      <c r="I15" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="15">
-        <v>10</v>
-      </c>
-      <c r="J15" s="17">
+      <c r="J15" s="15">
+        <v>10</v>
+      </c>
+      <c r="K15" s="17">
         <v>10000</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="L15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="L15" s="17">
+      <c r="M15" s="17">
         <v>200</v>
       </c>
-      <c r="M15" s="17">
+      <c r="N15" s="17">
         <v>50</v>
       </c>
-      <c r="N15" s="17">
+      <c r="O15" s="17">
         <v>2</v>
       </c>
-      <c r="O15" s="15">
-        <v>10</v>
-      </c>
       <c r="P15" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q15" s="19">
+      <c r="R15" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R15" s="20">
+      <c r="S15" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:19">
       <c r="A16" s="13" t="s">
         <v>59</v>
       </c>
@@ -2853,50 +2875,51 @@
       <c r="E16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="22">
-        <v>1196295513</v>
-      </c>
+      <c r="F16" s="21"/>
       <c r="G16" s="22">
         <v>1196295513</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="22">
+        <v>1196295513</v>
+      </c>
+      <c r="I16" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="15">
-        <v>10</v>
-      </c>
-      <c r="J16" s="17">
+      <c r="J16" s="15">
+        <v>10</v>
+      </c>
+      <c r="K16" s="17">
         <v>10000</v>
       </c>
-      <c r="K16" s="18" t="s">
+      <c r="L16" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="17">
+      <c r="M16" s="17">
         <v>200</v>
       </c>
-      <c r="M16" s="17">
+      <c r="N16" s="17">
         <v>50</v>
       </c>
-      <c r="N16" s="17">
+      <c r="O16" s="17">
         <v>2</v>
       </c>
-      <c r="O16" s="15">
-        <v>10</v>
-      </c>
       <c r="P16" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q16" s="19">
+      <c r="R16" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R16" s="20">
+      <c r="S16" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:19">
       <c r="A17" s="23" t="s">
         <v>18</v>
       </c>
@@ -2910,51 +2933,52 @@
       <c r="E17" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="25">
-        <v>1206274707</v>
-      </c>
+      <c r="F17" s="24"/>
       <c r="G17" s="25">
         <v>1206274707</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="25">
+        <v>1206274707</v>
+      </c>
+      <c r="I17" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="25">
-        <v>10</v>
-      </c>
-      <c r="J17" s="27">
-        <f>I17*1000</f>
+      <c r="J17" s="25">
+        <v>10</v>
+      </c>
+      <c r="K17" s="27">
+        <f>J17*1000</f>
         <v>10000</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="L17" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="27">
+      <c r="M17" s="27">
         <v>200</v>
       </c>
-      <c r="M17" s="27">
+      <c r="N17" s="27">
         <v>50</v>
       </c>
-      <c r="N17" s="27">
+      <c r="O17" s="27">
         <v>2</v>
       </c>
-      <c r="O17" s="25">
-        <v>10</v>
-      </c>
       <c r="P17" s="25">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="25">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q17" s="29">
+      <c r="R17" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R17" s="30">
+      <c r="S17" s="30">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:19">
       <c r="A18" s="5" t="s">
         <v>63</v>
       </c>
@@ -2966,50 +2990,51 @@
       <c r="E18" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="36">
-        <v>1196295489</v>
-      </c>
+      <c r="F18" s="35"/>
       <c r="G18" s="36">
         <v>1196295489</v>
       </c>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="36">
+        <v>1196295489</v>
+      </c>
+      <c r="I18" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="I18" s="7">
-        <v>10</v>
-      </c>
-      <c r="J18" s="9">
+      <c r="J18" s="7">
+        <v>10</v>
+      </c>
+      <c r="K18" s="9">
         <v>10000</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="L18" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="L18" s="9">
+      <c r="M18" s="9">
         <v>200</v>
       </c>
-      <c r="M18" s="9">
+      <c r="N18" s="9">
         <v>50</v>
       </c>
-      <c r="N18" s="9">
+      <c r="O18" s="9">
         <v>2</v>
       </c>
-      <c r="O18" s="7">
-        <v>10</v>
-      </c>
       <c r="P18" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="7">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q18" s="11">
+      <c r="R18" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R18" s="12">
+      <c r="S18" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:19">
       <c r="A19" s="13" t="s">
         <v>66</v>
       </c>
@@ -3021,50 +3046,51 @@
       <c r="E19" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="22">
-        <v>1196295443</v>
-      </c>
+      <c r="F19" s="21"/>
       <c r="G19" s="22">
         <v>1196295443</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="22">
+        <v>1196295443</v>
+      </c>
+      <c r="I19" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I19" s="15">
-        <v>10</v>
-      </c>
-      <c r="J19" s="17">
+      <c r="J19" s="15">
+        <v>10</v>
+      </c>
+      <c r="K19" s="17">
         <v>10000</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="L19" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="L19" s="17">
+      <c r="M19" s="17">
         <v>200</v>
       </c>
-      <c r="M19" s="17">
+      <c r="N19" s="17">
         <v>50</v>
       </c>
-      <c r="N19" s="17">
+      <c r="O19" s="17">
         <v>2</v>
       </c>
-      <c r="O19" s="15">
-        <v>10</v>
-      </c>
       <c r="P19" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q19" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q19" s="19">
+      <c r="R19" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R19" s="20">
+      <c r="S19" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:19">
       <c r="A20" s="13" t="s">
         <v>69</v>
       </c>
@@ -3076,50 +3102,51 @@
       <c r="E20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="22">
-        <v>1196295451</v>
-      </c>
+      <c r="F20" s="21"/>
       <c r="G20" s="22">
         <v>1196295451</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="22">
+        <v>1196295451</v>
+      </c>
+      <c r="I20" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="15">
-        <v>10</v>
-      </c>
-      <c r="J20" s="17">
+      <c r="J20" s="15">
+        <v>10</v>
+      </c>
+      <c r="K20" s="17">
         <v>10000</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="L20" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="L20" s="17">
+      <c r="M20" s="17">
         <v>200</v>
       </c>
-      <c r="M20" s="17">
+      <c r="N20" s="17">
         <v>50</v>
       </c>
-      <c r="N20" s="17">
+      <c r="O20" s="17">
         <v>2</v>
       </c>
-      <c r="O20" s="15">
-        <v>10</v>
-      </c>
       <c r="P20" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q20" s="19">
+      <c r="R20" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R20" s="20">
+      <c r="S20" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:19">
       <c r="A21" s="13" t="s">
         <v>72</v>
       </c>
@@ -3131,50 +3158,51 @@
       <c r="E21" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="22">
-        <v>1196295459</v>
-      </c>
+      <c r="F21" s="21"/>
       <c r="G21" s="22">
         <v>1196295459</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="22">
+        <v>1196295459</v>
+      </c>
+      <c r="I21" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="I21" s="15">
-        <v>10</v>
-      </c>
-      <c r="J21" s="17">
+      <c r="J21" s="15">
+        <v>10</v>
+      </c>
+      <c r="K21" s="17">
         <v>10000</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="L21" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="L21" s="17">
+      <c r="M21" s="17">
         <v>200</v>
       </c>
-      <c r="M21" s="17">
+      <c r="N21" s="17">
         <v>50</v>
       </c>
-      <c r="N21" s="17">
+      <c r="O21" s="17">
         <v>2</v>
       </c>
-      <c r="O21" s="15">
-        <v>10</v>
-      </c>
       <c r="P21" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q21" s="19">
+      <c r="R21" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R21" s="20">
+      <c r="S21" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:19">
       <c r="A22" s="13" t="s">
         <v>18</v>
       </c>
@@ -3188,51 +3216,52 @@
       <c r="E22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="15">
-        <v>1206274707</v>
-      </c>
+      <c r="F22" s="14"/>
       <c r="G22" s="15">
         <v>1206274707</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="15">
+        <v>1206274707</v>
+      </c>
+      <c r="I22" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="15">
-        <v>10</v>
-      </c>
-      <c r="J22" s="17">
-        <f>I22*1000</f>
+      <c r="J22" s="15">
+        <v>10</v>
+      </c>
+      <c r="K22" s="17">
+        <f>J22*1000</f>
         <v>10000</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="L22" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="L22" s="17">
+      <c r="M22" s="17">
         <v>200</v>
       </c>
-      <c r="M22" s="17">
+      <c r="N22" s="17">
         <v>50</v>
       </c>
-      <c r="N22" s="17">
+      <c r="O22" s="17">
         <v>2</v>
       </c>
-      <c r="O22" s="15">
-        <v>10</v>
-      </c>
       <c r="P22" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q22" s="19">
+      <c r="R22" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R22" s="20">
+      <c r="S22" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:19">
       <c r="A23" s="13" t="s">
         <v>18</v>
       </c>
@@ -3246,51 +3275,52 @@
       <c r="E23" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="15">
-        <v>1206274707</v>
-      </c>
+      <c r="F23" s="14"/>
       <c r="G23" s="15">
         <v>1206274707</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="15">
+        <v>1206274707</v>
+      </c>
+      <c r="I23" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="15">
-        <v>10</v>
-      </c>
-      <c r="J23" s="17">
-        <f>I23*1000</f>
+      <c r="J23" s="15">
+        <v>10</v>
+      </c>
+      <c r="K23" s="17">
+        <f>J23*1000</f>
         <v>10000</v>
       </c>
-      <c r="K23" s="18" t="s">
+      <c r="L23" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="L23" s="17">
+      <c r="M23" s="17">
         <v>200</v>
       </c>
-      <c r="M23" s="17">
+      <c r="N23" s="17">
         <v>20</v>
       </c>
-      <c r="N23" s="17">
+      <c r="O23" s="17">
         <v>2</v>
       </c>
-      <c r="O23" s="15">
-        <v>10</v>
-      </c>
       <c r="P23" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q23" s="19">
+      <c r="R23" s="19">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="R23" s="20">
+      <c r="S23" s="20">
         <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:19">
       <c r="A24" s="13" t="s">
         <v>38</v>
       </c>
@@ -3304,50 +3334,51 @@
       <c r="E24" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="15">
-        <v>1196295269</v>
-      </c>
+      <c r="F24" s="14"/>
       <c r="G24" s="15">
         <v>1196295269</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="15">
+        <v>1196295269</v>
+      </c>
+      <c r="I24" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="15">
-        <v>10</v>
-      </c>
-      <c r="J24" s="17">
+      <c r="J24" s="15">
+        <v>10</v>
+      </c>
+      <c r="K24" s="17">
         <v>10000</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="L24" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="L24" s="17">
+      <c r="M24" s="17">
         <v>200</v>
       </c>
-      <c r="M24" s="17">
+      <c r="N24" s="17">
         <v>50</v>
       </c>
-      <c r="N24" s="17">
+      <c r="O24" s="17">
         <v>2</v>
       </c>
-      <c r="O24" s="15">
-        <v>10</v>
-      </c>
       <c r="P24" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q24" s="19">
+      <c r="R24" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R24" s="20">
+      <c r="S24" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:19">
       <c r="A25" s="37" t="s">
         <v>40</v>
       </c>
@@ -3361,51 +3392,52 @@
       <c r="E25" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="39">
-        <v>1196295277</v>
-      </c>
+      <c r="F25" s="38"/>
       <c r="G25" s="39">
         <v>1196295277</v>
       </c>
-      <c r="H25" s="38" t="s">
+      <c r="H25" s="39">
+        <v>1196295277</v>
+      </c>
+      <c r="I25" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I25" s="39">
-        <v>10</v>
-      </c>
-      <c r="J25" s="41">
-        <f>I25*1000</f>
+      <c r="J25" s="39">
+        <v>10</v>
+      </c>
+      <c r="K25" s="41">
+        <f>J25*1000</f>
         <v>10000</v>
       </c>
-      <c r="K25" s="42" t="s">
+      <c r="L25" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="L25" s="41">
+      <c r="M25" s="41">
         <v>200</v>
       </c>
-      <c r="M25" s="41">
+      <c r="N25" s="41">
         <v>50</v>
       </c>
-      <c r="N25" s="41">
+      <c r="O25" s="41">
         <v>2</v>
       </c>
-      <c r="O25" s="39">
-        <v>10</v>
-      </c>
       <c r="P25" s="39">
+        <v>10</v>
+      </c>
+      <c r="Q25" s="39">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q25" s="43">
+      <c r="R25" s="43">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R25" s="44">
+      <c r="S25" s="44">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:19">
       <c r="A26" s="45" t="s">
         <v>43</v>
       </c>
@@ -3419,50 +3451,51 @@
       <c r="E26" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="47">
-        <v>1196295474</v>
-      </c>
+      <c r="F26" s="46"/>
       <c r="G26" s="47">
         <v>1196295474</v>
       </c>
-      <c r="H26" s="46" t="s">
+      <c r="H26" s="47">
+        <v>1196295474</v>
+      </c>
+      <c r="I26" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="47">
-        <v>10</v>
-      </c>
-      <c r="J26" s="49">
+      <c r="J26" s="47">
+        <v>10</v>
+      </c>
+      <c r="K26" s="49">
         <v>10000</v>
       </c>
-      <c r="K26" s="50" t="s">
+      <c r="L26" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="L26" s="49">
+      <c r="M26" s="49">
         <v>200</v>
       </c>
-      <c r="M26" s="49">
-        <v>10</v>
-      </c>
       <c r="N26" s="49">
+        <v>10</v>
+      </c>
+      <c r="O26" s="49">
         <v>2</v>
       </c>
-      <c r="O26" s="47">
-        <v>10</v>
-      </c>
       <c r="P26" s="47">
+        <v>10</v>
+      </c>
+      <c r="Q26" s="47">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q26" s="51">
+      <c r="R26" s="51">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="R26" s="52">
+      <c r="S26" s="52">
         <f t="shared" si="2"/>
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:19">
       <c r="A27" s="53" t="s">
         <v>46</v>
       </c>
@@ -3474,50 +3507,51 @@
       <c r="E27" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="22">
-        <v>1196295482</v>
-      </c>
+      <c r="F27" s="21"/>
       <c r="G27" s="22">
         <v>1196295482</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="22">
+        <v>1196295482</v>
+      </c>
+      <c r="I27" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="I27" s="15">
-        <v>10</v>
-      </c>
-      <c r="J27" s="17">
+      <c r="J27" s="15">
+        <v>10</v>
+      </c>
+      <c r="K27" s="17">
         <v>10000</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="L27" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="L27" s="17">
+      <c r="M27" s="17">
         <v>200</v>
       </c>
-      <c r="M27" s="17">
+      <c r="N27" s="17">
         <v>50</v>
       </c>
-      <c r="N27" s="17">
+      <c r="O27" s="17">
         <v>2</v>
       </c>
-      <c r="O27" s="15">
-        <v>10</v>
-      </c>
       <c r="P27" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q27" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q27" s="19">
+      <c r="R27" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R27" s="54">
+      <c r="S27" s="54">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:19">
       <c r="A28" s="53" t="s">
         <v>18</v>
       </c>
@@ -3531,51 +3565,52 @@
       <c r="E28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="15">
-        <v>1206274707</v>
-      </c>
+      <c r="F28" s="14"/>
       <c r="G28" s="15">
         <v>1206274707</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="15">
+        <v>1206274707</v>
+      </c>
+      <c r="I28" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="15">
-        <v>10</v>
-      </c>
-      <c r="J28" s="17">
-        <f>I28*1000</f>
+      <c r="J28" s="15">
+        <v>10</v>
+      </c>
+      <c r="K28" s="17">
+        <f>J28*1000</f>
         <v>10000</v>
       </c>
-      <c r="K28" s="18" t="s">
+      <c r="L28" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="L28" s="17">
+      <c r="M28" s="17">
         <v>200</v>
       </c>
-      <c r="M28" s="17">
+      <c r="N28" s="17">
         <v>50</v>
       </c>
-      <c r="N28" s="17">
+      <c r="O28" s="17">
         <v>2</v>
       </c>
-      <c r="O28" s="15">
-        <v>10</v>
-      </c>
       <c r="P28" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q28" s="19">
+      <c r="R28" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R28" s="54">
+      <c r="S28" s="54">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:19">
       <c r="A29" s="53" t="s">
         <v>50</v>
       </c>
@@ -3587,50 +3622,51 @@
       <c r="E29" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="22">
-        <v>1196295490</v>
-      </c>
+      <c r="F29" s="21"/>
       <c r="G29" s="22">
         <v>1196295490</v>
       </c>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="22">
+        <v>1196295490</v>
+      </c>
+      <c r="I29" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I29" s="15">
-        <v>10</v>
-      </c>
-      <c r="J29" s="17">
+      <c r="J29" s="15">
+        <v>10</v>
+      </c>
+      <c r="K29" s="17">
         <v>10000</v>
       </c>
-      <c r="K29" s="18" t="s">
+      <c r="L29" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="L29" s="17">
+      <c r="M29" s="17">
         <v>200</v>
       </c>
-      <c r="M29" s="17">
+      <c r="N29" s="17">
         <v>50</v>
       </c>
-      <c r="N29" s="17">
+      <c r="O29" s="17">
         <v>2</v>
       </c>
-      <c r="O29" s="15">
-        <v>10</v>
-      </c>
       <c r="P29" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q29" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q29" s="19">
+      <c r="R29" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R29" s="54">
+      <c r="S29" s="54">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:19">
       <c r="A30" s="53" t="s">
         <v>53</v>
       </c>
@@ -3642,50 +3678,51 @@
       <c r="E30" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="22">
-        <v>1196295522</v>
-      </c>
+      <c r="F30" s="21"/>
       <c r="G30" s="22">
         <v>1196295522</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="22">
+        <v>1196295522</v>
+      </c>
+      <c r="I30" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I30" s="15">
-        <v>10</v>
-      </c>
-      <c r="J30" s="17">
+      <c r="J30" s="15">
+        <v>10</v>
+      </c>
+      <c r="K30" s="17">
         <v>10000</v>
       </c>
-      <c r="K30" s="18" t="s">
+      <c r="L30" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="L30" s="17">
+      <c r="M30" s="17">
         <v>200</v>
       </c>
-      <c r="M30" s="17">
+      <c r="N30" s="17">
         <v>50</v>
       </c>
-      <c r="N30" s="17">
+      <c r="O30" s="17">
         <v>2</v>
       </c>
-      <c r="O30" s="15">
-        <v>10</v>
-      </c>
       <c r="P30" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q30" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q30" s="19">
+      <c r="R30" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R30" s="54">
+      <c r="S30" s="54">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:19">
       <c r="A31" s="53" t="s">
         <v>56</v>
       </c>
@@ -3697,50 +3734,51 @@
       <c r="E31" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="22">
-        <v>1196295506</v>
-      </c>
+      <c r="F31" s="21"/>
       <c r="G31" s="22">
         <v>1196295506</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="22">
+        <v>1196295506</v>
+      </c>
+      <c r="I31" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I31" s="15">
-        <v>10</v>
-      </c>
-      <c r="J31" s="17">
+      <c r="J31" s="15">
+        <v>10</v>
+      </c>
+      <c r="K31" s="17">
         <v>10000</v>
       </c>
-      <c r="K31" s="18" t="s">
+      <c r="L31" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="L31" s="17">
+      <c r="M31" s="17">
         <v>200</v>
       </c>
-      <c r="M31" s="17">
+      <c r="N31" s="17">
         <v>50</v>
       </c>
-      <c r="N31" s="17">
+      <c r="O31" s="17">
         <v>2</v>
       </c>
-      <c r="O31" s="15">
-        <v>10</v>
-      </c>
       <c r="P31" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q31" s="19">
+      <c r="R31" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R31" s="54">
+      <c r="S31" s="54">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:19">
       <c r="A32" s="53" t="s">
         <v>59</v>
       </c>
@@ -3752,50 +3790,51 @@
       <c r="E32" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="22">
-        <v>1196295513</v>
-      </c>
+      <c r="F32" s="21"/>
       <c r="G32" s="22">
         <v>1196295513</v>
       </c>
-      <c r="H32" s="21" t="s">
+      <c r="H32" s="22">
+        <v>1196295513</v>
+      </c>
+      <c r="I32" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="I32" s="15">
-        <v>10</v>
-      </c>
-      <c r="J32" s="17">
+      <c r="J32" s="15">
+        <v>10</v>
+      </c>
+      <c r="K32" s="17">
         <v>10000</v>
       </c>
-      <c r="K32" s="18" t="s">
+      <c r="L32" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L32" s="17">
+      <c r="M32" s="17">
         <v>200</v>
       </c>
-      <c r="M32" s="17">
+      <c r="N32" s="17">
         <v>50</v>
       </c>
-      <c r="N32" s="17">
+      <c r="O32" s="17">
         <v>2</v>
       </c>
-      <c r="O32" s="15">
-        <v>10</v>
-      </c>
       <c r="P32" s="15">
+        <v>10</v>
+      </c>
+      <c r="Q32" s="15">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q32" s="19">
+      <c r="R32" s="19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R32" s="54">
+      <c r="S32" s="54">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:19">
       <c r="A33" s="55" t="s">
         <v>18</v>
       </c>
@@ -3809,46 +3848,47 @@
       <c r="E33" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="39">
-        <v>1206274707</v>
-      </c>
+      <c r="F33" s="38"/>
       <c r="G33" s="39">
         <v>1206274707</v>
       </c>
-      <c r="H33" s="38" t="s">
+      <c r="H33" s="39">
+        <v>1206274707</v>
+      </c>
+      <c r="I33" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I33" s="39">
-        <v>10</v>
-      </c>
-      <c r="J33" s="41">
-        <f>I33*1000</f>
+      <c r="J33" s="39">
+        <v>10</v>
+      </c>
+      <c r="K33" s="41">
+        <f>J33*1000</f>
         <v>10000</v>
       </c>
-      <c r="K33" s="42" t="s">
+      <c r="L33" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="L33" s="41">
+      <c r="M33" s="41">
         <v>200</v>
       </c>
-      <c r="M33" s="41">
+      <c r="N33" s="41">
         <v>50</v>
       </c>
-      <c r="N33" s="41">
+      <c r="O33" s="41">
         <v>2</v>
       </c>
-      <c r="O33" s="39">
-        <v>10</v>
-      </c>
       <c r="P33" s="39">
+        <v>10</v>
+      </c>
+      <c r="Q33" s="39">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="Q33" s="43">
+      <c r="R33" s="43">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R33" s="56">
+      <c r="S33" s="56">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>

</xml_diff>